<commit_message>
test of pagina het deed
</commit_message>
<xml_diff>
--- a/Documenten/logboekFotosjaak.xlsx
+++ b/Documenten/logboekFotosjaak.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Logboek</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Begin gemaaktaan de MySqlDatabaseClass</t>
+  </si>
+  <si>
+    <t>Kijken of de Class werkt</t>
   </si>
 </sst>
 </file>
@@ -820,7 +823,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F12:F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,15 +1009,21 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="C12" s="9">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="E12" s="8">
         <v>6</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="G12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222099E-3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1169,7 +1178,7 @@
       </c>
       <c r="G26" s="9">
         <f>SUM(G7:G22)</f>
-        <v>6.8749999999999978E-2</v>
+        <v>7.2222222222222188E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test script login gemaakt
</commit_message>
<xml_diff>
--- a/Documenten/logboekFotosjaak.xlsx
+++ b/Documenten/logboekFotosjaak.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="28185" windowHeight="11130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28185" windowHeight="10710" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 47" sheetId="1" r:id="rId1"/>
     <sheet name="week 48" sheetId="2" r:id="rId2"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId3"/>
+    <sheet name="week 50" sheetId="5" r:id="rId3"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <oleSize ref="A1:V32"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A1:V29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Logboek</t>
   </si>
@@ -101,6 +102,12 @@
   </si>
   <si>
     <t>LoginClass verdergenaakt, er zijn 2 functions toegevoegd en kan verbinding maken met de mysqldatabaseclass.</t>
+  </si>
+  <si>
+    <t>Donnderdag</t>
+  </si>
+  <si>
+    <t>Heb de Login Class test script gemaakt</t>
   </si>
 </sst>
 </file>
@@ -110,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +206,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -246,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,23 +506,23 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="2"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.75" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -520,7 +530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -528,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -536,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -560,7 +570,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.5">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -585,7 +595,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -606,7 +616,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9"/>
@@ -621,7 +631,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9"/>
@@ -636,7 +646,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="9"/>
@@ -651,7 +661,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9"/>
@@ -665,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9"/>
@@ -679,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8">
@@ -691,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8">
@@ -703,14 +713,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8">
@@ -722,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -734,14 +744,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -754,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -766,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -779,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -789,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -799,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -809,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
@@ -831,19 +841,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="3"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,7 +861,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -862,7 +872,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -873,7 +883,7 @@
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -884,12 +894,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -913,7 +923,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -938,7 +948,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -959,7 +969,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="42.75">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9">
@@ -980,7 +990,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9"/>
@@ -990,7 +1000,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1025,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9">
@@ -1035,7 +1045,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9">
@@ -1055,7 +1065,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="C14" s="9">
         <v>0.47222222222222227</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>2.7777777777777735E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="42.75">
       <c r="C15" s="9">
         <v>0.5</v>
       </c>
@@ -1091,14 +1101,14 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8">
@@ -1110,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -1122,14 +1132,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1142,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -1154,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -1167,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1177,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -1187,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1197,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -1215,25 +1225,365 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41620</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9">
+        <f>D7-C7</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9">
+        <f t="shared" ref="G8:G18" si="0">D8-C8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8">
+        <v>6</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8">
+        <v>8</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="8">
+        <v>9</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8">
+        <v>10</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8">
+        <v>11</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8">
+        <v>12</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="9">
+        <f t="shared" ref="G20:G25" si="1">D20-C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8">
+        <v>13</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8">
+        <v>14</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9">
+        <f>SUM(G7:G22)</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1243,7 +1593,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1603,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1263,7 +1613,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -1271,7 +1621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="3">
         <v>47</v>
       </c>
@@ -1280,13 +1630,13 @@
         <v>6.5972222222222265E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>48</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
SessionClass gemaakt en geincluded bij connect_db
</commit_message>
<xml_diff>
--- a/Documenten/logboekFotosjaak.xlsx
+++ b/Documenten/logboekFotosjaak.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projecten\blok2\FotoSjaak\Documenten\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="2"/>
   </bookViews>
@@ -13,12 +18,11 @@
     <sheet name="Totaal" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:V29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t>Logboek</t>
   </si>
@@ -111,6 +115,9 @@
   </si>
   <si>
     <t>Bug Fixes</t>
+  </si>
+  <si>
+    <t>SessionClass gemaakt en aanpasingen gedaan in de connect_db</t>
   </si>
 </sst>
 </file>
@@ -1345,14 +1352,9 @@
       <c r="B8" s="3"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="8">
-        <v>2</v>
-      </c>
+      <c r="E8" s="8"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="9">
-        <f t="shared" ref="G8:G18" si="0">D8-C8</f>
-        <v>0</v>
-      </c>
+      <c r="G8" s="9"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
@@ -1375,19 +1377,30 @@
         <v>30</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G8:G18" si="0">D9-C9</f>
         <v>4.8611111111111105E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="28.5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
@@ -1571,7 +1584,7 @@
       </c>
       <c r="G26" s="9">
         <f>SUM(G7:G22)</f>
-        <v>6.1111111111111116E-2</v>
+        <v>8.1944444444444431E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begonnen aan een nieuwe method
</commit_message>
<xml_diff>
--- a/Documenten/logboekFotosjaak.xlsx
+++ b/Documenten/logboekFotosjaak.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Logboek</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>SessionClass gemaakt en aanpasingen gedaan in de connect_db</t>
+  </si>
+  <si>
+    <t>begonnen aan een nieuwe method</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1244,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1377,7 +1380,7 @@
         <v>30</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ref="G8:G18" si="0">D9-C9</f>
+        <f t="shared" ref="G9:G18" si="0">D9-C9</f>
         <v>4.8611111111111105E-2</v>
       </c>
       <c r="H9" s="3"/>
@@ -1406,15 +1409,21 @@
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="9">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="E11" s="8">
         <v>5</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -1584,7 +1593,7 @@
       </c>
       <c r="G26" s="9">
         <f>SUM(G7:G22)</f>
-        <v>8.1944444444444431E-2</v>
+        <v>0.10625000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>